<commit_message>
move things around, address feedback
</commit_message>
<xml_diff>
--- a/example/report_2022_awv.xlsx
+++ b/example/report_2022_awv.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
   <si>
     <t>Meldezeitraum</t>
   </si>
@@ -41,18 +41,33 @@
     <t>Ausgehende Zahlungen</t>
   </si>
   <si>
+    <t>2022-10</t>
+  </si>
+  <si>
     <t>2022-9</t>
   </si>
   <si>
+    <t>Bonuserhalt in Form von Aktien aus RSUs (GOOG [FILL OUT FULL COMPANY NAME])</t>
+  </si>
+  <si>
     <t>Bonuserhalt in Form von Aktien aus RSUs (NVIDIA Corp.)</t>
   </si>
   <si>
+    <t>FILL OUT COUNTRY</t>
+  </si>
+  <si>
     <t>USA</t>
   </si>
   <si>
+    <t>FILL OUT COUNTRY CODE</t>
+  </si>
+  <si>
     <t>US</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
@@ -65,6 +80,21 @@
     <t>ISIN</t>
   </si>
   <si>
+    <t>2022-11</t>
+  </si>
+  <si>
+    <t>GOOG [FILL OUT FULL COMPANY NAME] (Erhalt Aktien aus RSUs)</t>
+  </si>
+  <si>
+    <t>GOOG [FILl OUT FULL COMPANY NAME] (Verkauf zur Erzielung dt. EkSt)</t>
+  </si>
+  <si>
+    <t>APPL [FILL OUT FULL COMPANY NAME] (Verkauf von Aktien aus RSUs/ESPP)</t>
+  </si>
+  <si>
+    <t>GOOG [FILL OUT FULL COMPANY NAME] (Verkauf von Aktien aus RSUs/ESPP)</t>
+  </si>
+  <si>
     <t>NVIDIA Corp. (Verkauf von Aktien aus RSUs/ESPP)</t>
   </si>
   <si>
@@ -74,7 +104,13 @@
     <t>NVIDIA Corp. (Verkauf zur Erzielung dt. EkSt.)</t>
   </si>
   <si>
+    <t>FILL OUT ISIN</t>
+  </si>
+  <si>
     <t>US67066G1040</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>3</t>
@@ -438,18 +474,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -485,7 +521,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -494,13 +530,36 @@
         <v>521</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>521</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -515,7 +574,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -524,10 +583,10 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -540,13 +599,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -569,22 +628,22 @@
         <v>104</v>
       </c>
       <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -595,27 +654,27 @@
         <v>104</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>104</v>
@@ -624,71 +683,227 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>104</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>104</v>
       </c>
       <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>104</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>104</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>104</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>104</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>104</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>104</v>
+      </c>
+      <c r="C12">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
forgot to commit pieces, commit local progress now
</commit_message>
<xml_diff>
--- a/example/report_2022_awv.xlsx
+++ b/example/report_2022_awv.xlsx
@@ -641,7 +641,7 @@
         <v>104</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -844,7 +844,7 @@
         <v>104</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>

</xml_diff>